<commit_message>
Including all templates for dutch in the template
</commit_message>
<xml_diff>
--- a/BaseFiles/2_Closing_0.xlsx
+++ b/BaseFiles/2_Closing_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hostbv833-my.sharepoint.com/personal/g_vandoorn_bright-renewables_com/Documents/Documenten/Python Scripts/BURP/BaseFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_F25DC773A252ABDACC10483F519C5AEC5ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A909EDCE-8BC9-475B-BD76-D23C4CFA4C67}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ABA72D9-25D9-4963-BFAE-9CD42FF8493B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Overzicht en analyse niet geplande interventies</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Overzicht van geplande interventies</t>
   </si>
   <si>
-    <t>wisseling actief kool</t>
-  </si>
-  <si>
     <t>H2S-kool</t>
   </si>
   <si>
@@ -55,6 +52,24 @@
   </si>
   <si>
     <t>VOC-kool</t>
+  </si>
+  <si>
+    <t>Actiepunten</t>
+  </si>
+  <si>
+    <t>omschrijving</t>
+  </si>
+  <si>
+    <t>actiehouder</t>
+  </si>
+  <si>
+    <t>einddatum</t>
+  </si>
+  <si>
+    <t>Wisselingen gasflessen, THT</t>
+  </si>
+  <si>
+    <t>Wisseling actief kool</t>
   </si>
 </sst>
 </file>
@@ -201,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -214,9 +229,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,8 +636,8 @@
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
-        <v>6</v>
+      <c r="A18" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -628,27 +648,107 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" t="s">
         <v>7</v>
-      </c>
-      <c r="B19" s="13"/>
-      <c r="C19" t="s">
-        <v>8</v>
       </c>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="14"/>
+        <v>8</v>
+      </c>
+      <c r="B20" s="13"/>
       <c r="C20" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="11"/>
     </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="17"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="E28" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>